<commit_message>
update plots for each sample
</commit_message>
<xml_diff>
--- a/validation/results/20210618-630039/20210618-630039.xlsx
+++ b/validation/results/20210618-630039/20210618-630039.xlsx
@@ -4316,7 +4316,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>GG</t>
+          <t>G</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -4400,7 +4400,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>TT</t>
+          <t>T</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -4442,7 +4442,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>GG</t>
+          <t>G</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -4484,7 +4484,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>GG</t>
+          <t>G</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -4526,7 +4526,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>GG</t>
+          <t>G</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -4568,7 +4568,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>GG</t>
+          <t>G</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -4610,7 +4610,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>TT</t>
+          <t>T</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -4652,7 +4652,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>GG</t>
+          <t>G</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -4736,7 +4736,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>GG</t>
+          <t>G</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -4778,7 +4778,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -4820,7 +4820,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -4862,7 +4862,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -4904,7 +4904,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>TT</t>
+          <t>T</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -4946,7 +4946,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>GG</t>
+          <t>G</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>GG</t>
+          <t>G</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -5034,7 +5034,11 @@
           <t>20210618-630039</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>*2/*5</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>